<commit_message>
start updating the examples
</commit_message>
<xml_diff>
--- a/examples/reports/example1.xlsx
+++ b/examples/reports/example1.xlsx
@@ -17,9 +17,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -36,6 +37,13 @@
     <font>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -66,13 +74,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -443,49 +463,56 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="A1:C2"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="20.7" customWidth="1" style="3" min="1" max="1"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="12.8" customHeight="1" s="4">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Author</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="1">
-      <c r="A2" s="2" t="inlineStr">
+    <row r="2" ht="12.8" customHeight="1" s="4">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>Water Discharge Report</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>JOHN DOE</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>January 1st, 2023</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>